<commit_message>
Added Product Edit API
</commit_message>
<xml_diff>
--- a/data/OnlineStoreAppDatabase.xlsx
+++ b/data/OnlineStoreAppDatabase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OnlineStoreAppBackendAPI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6865762-3682-4E35-A40D-CBA9FB9AFF08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25401B8F-AF04-41AB-9B87-42305B95F564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{78640D3A-98CE-471C-B44F-E0F00B51329B}"/>
+    <workbookView xWindow="432" yWindow="24" windowWidth="19500" windowHeight="11508" activeTab="2" xr2:uid="{78640D3A-98CE-471C-B44F-E0F00B51329B}"/>
   </bookViews>
   <sheets>
     <sheet name="Managers" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="172">
   <si>
     <t>Email</t>
   </si>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9D87FB-2A61-45A2-90B9-AC1E61A8CBD4}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98:B121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,18 +1100,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="5">
-        <v>1250</v>
-      </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="C2" t="n">
+        <v>1250.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10.0</v>
       </c>
       <c r="E2" t="s">
         <v>148</v>
@@ -1119,7 +1119,7 @@
       <c r="F2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3860,18 +3860,18 @@
         <v>156</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>167</v>
       </c>
       <c r="B122" t="s">
         <v>168</v>
       </c>
-      <c r="C122" t="n">
-        <v>1250.0</v>
-      </c>
-      <c r="D122" t="n">
-        <v>2.0</v>
+      <c r="C122">
+        <v>1250</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
       </c>
       <c r="E122" t="s">
         <v>151</v>
@@ -3883,18 +3883,18 @@
         <v>152</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>169</v>
       </c>
       <c r="B123" t="s">
         <v>168</v>
       </c>
-      <c r="C123" t="n">
-        <v>1500.0</v>
-      </c>
-      <c r="D123" t="n">
-        <v>2.0</v>
+      <c r="C123">
+        <v>1500</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
       </c>
       <c r="E123" t="s">
         <v>151</v>
@@ -3906,18 +3906,18 @@
         <v>152</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>170</v>
       </c>
       <c r="B124" t="s">
         <v>168</v>
       </c>
-      <c r="C124" t="n">
-        <v>1700.0</v>
-      </c>
-      <c r="D124" t="n">
-        <v>3.0</v>
+      <c r="C124">
+        <v>1700</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
       </c>
       <c r="E124" t="s">
         <v>151</v>
@@ -3929,18 +3929,18 @@
         <v>152</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>171</v>
       </c>
       <c r="B125" t="s">
         <v>168</v>
       </c>
-      <c r="C125" t="n">
-        <v>1700.0</v>
-      </c>
-      <c r="D125" t="n">
-        <v>3.0</v>
+      <c r="C125">
+        <v>1700</v>
+      </c>
+      <c r="D125">
+        <v>3</v>
       </c>
       <c r="E125" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Added API for edit customer
</commit_message>
<xml_diff>
--- a/data/OnlineStoreAppDatabase.xlsx
+++ b/data/OnlineStoreAppDatabase.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="176">
   <si>
     <t>Email</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>Patna</t>
+  </si>
+  <si>
+    <t>kishorekumar@gmail.com</t>
+  </si>
+  <si>
+    <t>Kishore kumar</t>
   </si>
 </sst>
 </file>
@@ -1075,13 +1081,13 @@
         <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
         <v>171</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added backend API's for customer signin and signout
</commit_message>
<xml_diff>
--- a/data/OnlineStoreAppDatabase.xlsx
+++ b/data/OnlineStoreAppDatabase.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="186">
   <si>
     <t>Email</t>
   </si>
@@ -555,6 +555,36 @@
   </si>
   <si>
     <t>Kishore kumar</t>
+  </si>
+  <si>
+    <t>C#00004</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>9935465163</t>
+  </si>
+  <si>
+    <t>amankumar@gmail.com</t>
+  </si>
+  <si>
+    <t>C#00005</t>
+  </si>
+  <si>
+    <t>9031398069</t>
+  </si>
+  <si>
+    <t>Pragathi Layout</t>
+  </si>
+  <si>
+    <t>C#00006</t>
+  </si>
+  <si>
+    <t>Abhi</t>
+  </si>
+  <si>
+    <t>abhi@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -990,7 +1020,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22289BA1-EEE9-47AF-89E2-B0A06405A6E0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -1030,47 +1060,47 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>173</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -1078,31 +1108,51 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>174</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{C3CE85AE-D2B4-46DE-99DD-9F6BD76B4177}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>

</xml_diff>